<commit_message>
Finish Lesson 6 - Normal Distribution
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToDescriptiveStats/Lesson5_Standardizing.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToDescriptiveStats/Lesson5_Standardizing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10110" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>0.2</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -562,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>205</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C4">
         <v>137</v>
@@ -607,55 +607,55 @@
       </c>
       <c r="B5">
         <f>(B4-$B$2)/$B$3</f>
-        <v>2.125</v>
+        <v>0.14999999999999902</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:N5" si="0">(C4-$B$2)/$B$3</f>
-        <v>0.42499999999999999</v>
+        <v>675</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-2.5</v>
+        <v>90</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>-0.75</v>
+        <v>440</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>-2.3624999999999998</v>
+        <v>117.5</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>-2.3374999999999999</v>
+        <v>122.5</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>-2.3125</v>
+        <v>127.5</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>-2.2875000000000001</v>
+        <v>132.5</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>-2.2625000000000002</v>
+        <v>137.5</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>-2.2374999999999998</v>
+        <v>142.5</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>-2.2124999999999999</v>
+        <v>147.5</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>-2.1875</v>
+        <v>152.5</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>-2.1625000000000001</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
       </c>
       <c r="F6">
         <f>(50-F5)/10</f>
-        <v>5.2362500000000001</v>
+        <v>-6.75</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.35">
@@ -736,9 +736,19 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f>1-0.5596</f>
+        <v>0.44040000000000001</v>
+      </c>
+    </row>
     <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="F14" s="2">
         <v>10</v>
+      </c>
+      <c r="K14">
+        <f>(1.83-2)/0.02</f>
+        <v>-8.4999999999999964</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.35">
@@ -789,7 +799,7 @@
         <v>0.5</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="B19:C19" si="1">(C18-C16)/C17</f>
+        <f t="shared" ref="C19" si="1">(C18-C16)/C17</f>
         <v>2</v>
       </c>
     </row>
@@ -803,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -851,13 +861,13 @@
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3">
-        <f>A2-$C$1</f>
+        <f t="shared" ref="D2:D33" si="0">A2-$C$1</f>
         <v>-31.828571428571422</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4">
-        <f>D2/$F$1</f>
+        <f t="shared" ref="G2:G33" si="1">D2/$F$1</f>
         <v>-2.134961660885383</v>
       </c>
       <c r="H2" s="4"/>
@@ -883,13 +893,13 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
-        <f>A3-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-26.828571428571422</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4">
-        <f>D3/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.7995771988971045</v>
       </c>
       <c r="H3" s="4"/>
@@ -915,13 +925,13 @@
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
-        <f>A4-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-26.828571428571422</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4">
-        <f>D4/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.7995771988971045</v>
       </c>
       <c r="H4" s="4"/>
@@ -947,13 +957,13 @@
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
-        <f>A5-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-21.828571428571422</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4">
-        <f>D5/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.4641927369088261</v>
       </c>
       <c r="H5" s="4"/>
@@ -980,13 +990,13 @@
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
-        <f>A6-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-19.828571428571422</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4">
-        <f>D6/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.3300389521135147</v>
       </c>
       <c r="H6" s="4"/>
@@ -1010,13 +1020,13 @@
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <f>A7-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-19.828571428571422</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4">
-        <f>D7/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.3300389521135147</v>
       </c>
       <c r="H7" s="4"/>
@@ -1056,13 +1066,13 @@
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <f>A8-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-18.828571428571422</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4">
-        <f>D8/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.2629620597158591</v>
       </c>
       <c r="H8" s="4"/>
@@ -1094,13 +1104,13 @@
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <f>A9-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-18.828571428571422</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4">
-        <f>D9/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.2629620597158591</v>
       </c>
       <c r="H9" s="4"/>
@@ -1133,13 +1143,13 @@
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <f>A10-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-18.828571428571422</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4">
-        <f>D10/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.2629620597158591</v>
       </c>
       <c r="H10" s="4"/>
@@ -1174,13 +1184,13 @@
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
-        <f>A11-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-17.828571428571422</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4">
-        <f>D11/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.1958851673182034</v>
       </c>
       <c r="H11" s="4"/>
@@ -1204,13 +1214,13 @@
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
-        <f>A12-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-17.828571428571422</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
-        <f>D12/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.1958851673182034</v>
       </c>
       <c r="H12" s="4"/>
@@ -1234,13 +1244,13 @@
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <f>A13-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-17.828571428571422</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4">
-        <f>D13/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.1958851673182034</v>
       </c>
       <c r="H13" s="4"/>
@@ -1264,13 +1274,13 @@
       <c r="B14" s="4"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
-        <f>A14-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-16.828571428571422</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4">
-        <f>D14/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.1288082749205477</v>
       </c>
       <c r="H14" s="4"/>
@@ -1294,13 +1304,13 @@
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <f>A15-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-16.828571428571422</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4">
-        <f>D15/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.1288082749205477</v>
       </c>
       <c r="H15" s="4"/>
@@ -1324,13 +1334,13 @@
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
-        <f>A16-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-15.828571428571422</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4">
-        <f>D16/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.0617313825228922</v>
       </c>
       <c r="H16" s="4"/>
@@ -1354,13 +1364,13 @@
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <f>A17-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-15.828571428571422</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4">
-        <f>D17/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-1.0617313825228922</v>
       </c>
       <c r="H17" s="4"/>
@@ -1384,13 +1394,13 @@
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
-        <f>A18-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-13.828571428571422</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4">
-        <f>D18/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.92757759772758075</v>
       </c>
       <c r="H18" s="4"/>
@@ -1414,13 +1424,13 @@
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
-        <f>A19-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-11.828571428571422</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4">
-        <f>D19/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.79342381293226949</v>
       </c>
       <c r="H19" s="4"/>
@@ -1444,13 +1454,13 @@
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
-        <f>A20-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-9.8285714285714221</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>D20/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.65927002813695812</v>
       </c>
       <c r="H20" s="4"/>
@@ -1474,13 +1484,13 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
-        <f>A21-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-8.8285714285714221</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="4">
-        <f>D21/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.59219313573930243</v>
       </c>
       <c r="H21" s="4"/>
@@ -1504,13 +1514,13 @@
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
-        <f>A22-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-8.8285714285714221</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4">
-        <f>D22/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.59219313573930243</v>
       </c>
       <c r="H22" s="4"/>
@@ -1534,13 +1544,13 @@
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3">
-        <f>A23-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-7.8285714285714221</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4">
-        <f>D23/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.52511624334164675</v>
       </c>
       <c r="H23" s="4"/>
@@ -1564,13 +1574,13 @@
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
-        <f>A24-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-7.8285714285714221</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4">
-        <f>D24/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.52511624334164675</v>
       </c>
       <c r="H24" s="4"/>
@@ -1594,13 +1604,13 @@
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
-        <f>A25-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-5.8285714285714221</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4">
-        <f>D25/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.39096245854633543</v>
       </c>
       <c r="H25" s="4"/>
@@ -1624,13 +1634,13 @@
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3">
-        <f>A26-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-4.8285714285714221</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4">
-        <f>D26/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.3238855661486798</v>
       </c>
       <c r="H26" s="4"/>
@@ -1654,13 +1664,13 @@
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3">
-        <f>A27-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-2.8285714285714221</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4">
-        <f>D27/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.18973178135336846</v>
       </c>
       <c r="H27" s="4"/>
@@ -1684,13 +1694,13 @@
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
-        <f>A28-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-2.8285714285714221</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4">
-        <f>D28/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.18973178135336846</v>
       </c>
       <c r="H28" s="4"/>
@@ -1714,13 +1724,13 @@
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
-        <f>A29-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-2.8285714285714221</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4">
-        <f>D29/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.18973178135336846</v>
       </c>
       <c r="H29" s="4"/>
@@ -1744,13 +1754,13 @@
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3">
-        <f>A30-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-2.8285714285714221</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4">
-        <f>D30/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.18973178135336846</v>
       </c>
       <c r="H30" s="4"/>
@@ -1774,13 +1784,13 @@
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3">
-        <f>A31-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-1.8285714285714221</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4">
-        <f>D31/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.12265488895571279</v>
       </c>
       <c r="H31" s="4"/>
@@ -1804,13 +1814,13 @@
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3">
-        <f>A32-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-1.8285714285714221</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4">
-        <f>D32/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-0.12265488895571279</v>
       </c>
       <c r="H32" s="4"/>
@@ -1834,13 +1844,13 @@
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3">
-        <f>A33-$C$1</f>
+        <f t="shared" si="0"/>
         <v>-0.82857142857142208</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4">
-        <f>D33/$F$1</f>
+        <f t="shared" si="1"/>
         <v>-5.5577996558057119E-2</v>
       </c>
       <c r="H33" s="4"/>
@@ -1864,13 +1874,13 @@
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3">
-        <f>A34-$C$1</f>
+        <f t="shared" ref="D34:D65" si="2">A34-$C$1</f>
         <v>-0.82857142857142208</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4">
-        <f>D34/$F$1</f>
+        <f t="shared" ref="G34:G65" si="3">D34/$F$1</f>
         <v>-5.5577996558057119E-2</v>
       </c>
       <c r="H34" s="4"/>
@@ -1894,13 +1904,13 @@
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3">
-        <f>A35-$C$1</f>
+        <f t="shared" si="2"/>
         <v>0.17142857142857792</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4">
-        <f>D35/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.1498895839598551E-2</v>
       </c>
       <c r="H35" s="4"/>
@@ -1924,13 +1934,13 @@
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3">
-        <f>A36-$C$1</f>
+        <f t="shared" si="2"/>
         <v>0.17142857142857792</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4">
-        <f>D36/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.1498895839598551E-2</v>
       </c>
       <c r="H36" s="4"/>
@@ -1954,13 +1964,13 @@
       <c r="B37" s="4"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <f>A37-$C$1</f>
+        <f t="shared" si="2"/>
         <v>0.17142857142857792</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4">
-        <f>D37/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.1498895839598551E-2</v>
       </c>
       <c r="H37" s="4"/>
@@ -1984,13 +1994,13 @@
       <c r="B38" s="4"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3">
-        <f>A38-$C$1</f>
+        <f t="shared" si="2"/>
         <v>1.1714285714285779</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4">
-        <f>D38/$F$1</f>
+        <f t="shared" si="3"/>
         <v>7.8575788237254224E-2</v>
       </c>
       <c r="H38" s="4"/>
@@ -2014,13 +2024,13 @@
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
-        <f>A39-$C$1</f>
+        <f t="shared" si="2"/>
         <v>2.1714285714285779</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4">
-        <f>D39/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.14565268063490988</v>
       </c>
       <c r="H39" s="4"/>
@@ -2044,13 +2054,13 @@
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3">
-        <f>A40-$C$1</f>
+        <f t="shared" si="2"/>
         <v>2.1714285714285779</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4">
-        <f>D40/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.14565268063490988</v>
       </c>
       <c r="H40" s="4"/>
@@ -2074,13 +2084,13 @@
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3">
-        <f>A41-$C$1</f>
+        <f t="shared" si="2"/>
         <v>3.1714285714285779</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4">
-        <f>D41/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.21272957303256554</v>
       </c>
       <c r="H41" s="4"/>
@@ -2104,13 +2114,13 @@
       <c r="B42" s="4"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
-        <f>A42-$C$1</f>
+        <f t="shared" si="2"/>
         <v>3.1714285714285779</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4">
-        <f>D42/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.21272957303256554</v>
       </c>
       <c r="H42" s="4"/>
@@ -2134,13 +2144,13 @@
       <c r="B43" s="4"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3">
-        <f>A43-$C$1</f>
+        <f t="shared" si="2"/>
         <v>3.1714285714285779</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4">
-        <f>D43/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.21272957303256554</v>
       </c>
       <c r="H43" s="4"/>
@@ -2164,13 +2174,13 @@
       <c r="B44" s="4"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3">
-        <f>A44-$C$1</f>
+        <f t="shared" si="2"/>
         <v>5.1714285714285779</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4">
-        <f>D44/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.34688335782787688</v>
       </c>
       <c r="H44" s="4"/>
@@ -2194,13 +2204,13 @@
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3">
-        <f>A45-$C$1</f>
+        <f t="shared" si="2"/>
         <v>5.1714285714285779</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4">
-        <f>D45/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.34688335782787688</v>
       </c>
       <c r="H45" s="4"/>
@@ -2224,13 +2234,13 @@
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3">
-        <f>A46-$C$1</f>
+        <f t="shared" si="2"/>
         <v>6.1714285714285779</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4">
-        <f>D46/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.41396025022553257</v>
       </c>
       <c r="H46" s="4"/>
@@ -2254,13 +2264,13 @@
       <c r="B47" s="4"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3">
-        <f>A47-$C$1</f>
+        <f t="shared" si="2"/>
         <v>6.1714285714285779</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4">
-        <f>D47/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.41396025022553257</v>
       </c>
       <c r="H47" s="4"/>
@@ -2284,13 +2294,13 @@
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3">
-        <f>A48-$C$1</f>
+        <f t="shared" si="2"/>
         <v>6.1714285714285779</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4">
-        <f>D48/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.41396025022553257</v>
       </c>
       <c r="H48" s="4"/>
@@ -2314,13 +2324,13 @@
       <c r="B49" s="4"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
-        <f>A49-$C$1</f>
+        <f t="shared" si="2"/>
         <v>7.1714285714285779</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4">
-        <f>D49/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.4810371426231882</v>
       </c>
       <c r="H49" s="4"/>
@@ -2344,13 +2354,13 @@
       <c r="B50" s="4"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3">
-        <f>A50-$C$1</f>
+        <f t="shared" si="2"/>
         <v>8.1714285714285779</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4">
-        <f>D50/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.54811403502084388</v>
       </c>
       <c r="H50" s="4"/>
@@ -2374,13 +2384,13 @@
       <c r="B51" s="4"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3">
-        <f>A51-$C$1</f>
+        <f t="shared" si="2"/>
         <v>8.1714285714285779</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4">
-        <f>D51/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.54811403502084388</v>
       </c>
       <c r="H51" s="4"/>
@@ -2404,13 +2414,13 @@
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3">
-        <f>A52-$C$1</f>
+        <f t="shared" si="2"/>
         <v>8.1714285714285779</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4">
-        <f>D52/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.54811403502084388</v>
       </c>
       <c r="H52" s="4"/>
@@ -2434,13 +2444,13 @@
       <c r="B53" s="4"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3">
-        <f>A53-$C$1</f>
+        <f t="shared" si="2"/>
         <v>9.1714285714285779</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4">
-        <f>D53/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.61519092741849957</v>
       </c>
       <c r="H53" s="4"/>
@@ -2464,13 +2474,13 @@
       <c r="B54" s="4"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3">
-        <f>A54-$C$1</f>
+        <f t="shared" si="2"/>
         <v>9.1714285714285779</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4">
-        <f>D54/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.61519092741849957</v>
       </c>
       <c r="H54" s="4"/>
@@ -2494,13 +2504,13 @@
       <c r="B55" s="4"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3">
-        <f>A55-$C$1</f>
+        <f t="shared" si="2"/>
         <v>9.1714285714285779</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4">
-        <f>D55/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.61519092741849957</v>
       </c>
       <c r="H55" s="4"/>
@@ -2524,13 +2534,13 @@
       <c r="B56" s="4"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3">
-        <f>A56-$C$1</f>
+        <f t="shared" si="2"/>
         <v>10.171428571428578</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4">
-        <f>D56/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.68226781981615525</v>
       </c>
       <c r="H56" s="4"/>
@@ -2554,13 +2564,13 @@
       <c r="B57" s="4"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3">
-        <f>A57-$C$1</f>
+        <f t="shared" si="2"/>
         <v>10.171428571428578</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4">
-        <f>D57/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.68226781981615525</v>
       </c>
       <c r="H57" s="4"/>
@@ -2584,13 +2594,13 @@
       <c r="B58" s="4"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3">
-        <f>A58-$C$1</f>
+        <f t="shared" si="2"/>
         <v>10.171428571428578</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4">
-        <f>D58/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.68226781981615525</v>
       </c>
       <c r="H58" s="4"/>
@@ -2614,13 +2624,13 @@
       <c r="B59" s="4"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3">
-        <f>A59-$C$1</f>
+        <f t="shared" si="2"/>
         <v>12.171428571428578</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4">
-        <f>D59/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.81642160461146651</v>
       </c>
       <c r="H59" s="4"/>
@@ -2644,13 +2654,13 @@
       <c r="B60" s="4"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3">
-        <f>A60-$C$1</f>
+        <f t="shared" si="2"/>
         <v>14.171428571428578</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4">
-        <f>D60/$F$1</f>
+        <f t="shared" si="3"/>
         <v>0.95057538940677788</v>
       </c>
       <c r="H60" s="4"/>
@@ -2674,13 +2684,13 @@
       <c r="B61" s="4"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3">
-        <f>A61-$C$1</f>
+        <f t="shared" si="2"/>
         <v>16.171428571428578</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4">
-        <f>D61/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.0847291742020893</v>
       </c>
       <c r="H61" s="4"/>
@@ -2704,13 +2714,13 @@
       <c r="B62" s="4"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3">
-        <f>A62-$C$1</f>
+        <f t="shared" si="2"/>
         <v>16.171428571428578</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4">
-        <f>D62/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.0847291742020893</v>
       </c>
       <c r="H62" s="4"/>
@@ -2734,13 +2744,13 @@
       <c r="B63" s="4"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3">
-        <f>A63-$C$1</f>
+        <f t="shared" si="2"/>
         <v>17.171428571428578</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4">
-        <f>D63/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.1518060665997449</v>
       </c>
       <c r="H63" s="4"/>
@@ -2764,13 +2774,13 @@
       <c r="B64" s="4"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3">
-        <f>A64-$C$1</f>
+        <f t="shared" si="2"/>
         <v>18.171428571428578</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4">
-        <f>D64/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.2188829589974006</v>
       </c>
       <c r="H64" s="4"/>
@@ -2794,13 +2804,13 @@
       <c r="B65" s="4"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3">
-        <f>A65-$C$1</f>
+        <f t="shared" si="2"/>
         <v>19.171428571428578</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4">
-        <f>D65/$F$1</f>
+        <f t="shared" si="3"/>
         <v>1.2859598513950563</v>
       </c>
       <c r="H65" s="4"/>
@@ -2824,13 +2834,13 @@
       <c r="B66" s="4"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3">
-        <f>A66-$C$1</f>
+        <f t="shared" ref="D66:D73" si="4">A66-$C$1</f>
         <v>22.171428571428578</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4">
-        <f>D66/$F$1</f>
+        <f t="shared" ref="G66:G73" si="5">D66/$F$1</f>
         <v>1.4871905285880231</v>
       </c>
       <c r="H66" s="4"/>
@@ -2854,13 +2864,13 @@
       <c r="B67" s="4"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3">
-        <f>A67-$C$1</f>
+        <f t="shared" si="4"/>
         <v>25.171428571428578</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4">
-        <f>D67/$F$1</f>
+        <f t="shared" si="5"/>
         <v>1.6884212057809902</v>
       </c>
       <c r="H67" s="4"/>
@@ -2884,13 +2894,13 @@
       <c r="B68" s="4"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3">
-        <f>A68-$C$1</f>
+        <f t="shared" si="4"/>
         <v>25.171428571428578</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4">
-        <f>D68/$F$1</f>
+        <f t="shared" si="5"/>
         <v>1.6884212057809902</v>
       </c>
       <c r="H68" s="4"/>
@@ -2914,13 +2924,13 @@
       <c r="B69" s="4"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3">
-        <f>A69-$C$1</f>
+        <f t="shared" si="4"/>
         <v>27.171428571428578</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4">
-        <f>D69/$F$1</f>
+        <f t="shared" si="5"/>
         <v>1.8225749905763016</v>
       </c>
       <c r="H69" s="4"/>
@@ -2944,13 +2954,13 @@
       <c r="B70" s="4"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3">
-        <f>A70-$C$1</f>
+        <f t="shared" si="4"/>
         <v>32.171428571428578</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4">
-        <f>D70/$F$1</f>
+        <f t="shared" si="5"/>
         <v>2.15795945256458</v>
       </c>
       <c r="H70" s="4"/>
@@ -2974,13 +2984,13 @@
       <c r="B71" s="4"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3">
-        <f>A71-$C$1</f>
+        <f t="shared" si="4"/>
         <v>39.171428571428578</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4">
-        <f>D71/$F$1</f>
+        <f t="shared" si="5"/>
         <v>2.6274976993481696</v>
       </c>
       <c r="H71" s="4"/>
@@ -3004,13 +3014,13 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4">
-        <f>A72-$C$1</f>
+        <f t="shared" si="4"/>
         <v>24.171428571428578</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4">
-        <f>D72/$F$1</f>
+        <f t="shared" si="5"/>
         <v>1.6213443133833345</v>
       </c>
       <c r="H72" s="4"/>
@@ -3034,13 +3044,13 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4">
-        <f>A73-$C$1</f>
+        <f t="shared" si="4"/>
         <v>49.171428571428578</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4">
-        <f>D73/$F$1</f>
+        <f t="shared" si="5"/>
         <v>3.2982666233247264</v>
       </c>
       <c r="H73" s="4"/>

</xml_diff>